<commit_message>
Controle atualização timezone relatórios
</commit_message>
<xml_diff>
--- a/Relatórios LN/Mapeamento_Reports.xlsx
+++ b/Relatórios LN/Mapeamento_Reports.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="122">
   <si>
     <t>View</t>
   </si>
@@ -244,13 +244,151 @@
   </si>
   <si>
     <t>DATA_FATURAMENTO</t>
+  </si>
+  <si>
+    <t>LN_FISCAL_Apuracao_imposto_federal_alt</t>
+  </si>
+  <si>
+    <t>DATA_LIQUIDACAO</t>
+  </si>
+  <si>
+    <t>LN_FISCAL_Apuracao_imposto_municipal</t>
+  </si>
+  <si>
+    <t>DT_NR</t>
+  </si>
+  <si>
+    <t>DT_VENC</t>
+  </si>
+  <si>
+    <t>LN_Gestão Financeira de Transporte - DBO_Etiquetas_Correios</t>
+  </si>
+  <si>
+    <t>não tem campo de data</t>
+  </si>
+  <si>
+    <t>LN_Inventario_Geral</t>
+  </si>
+  <si>
+    <t>LN_Itens_Cadastrados</t>
+  </si>
+  <si>
+    <t>DATA_INCLUSAO</t>
+  </si>
+  <si>
+    <t>DATA_ALTRERACAO</t>
+  </si>
+  <si>
+    <t>LN_Itens_Sem_OK_Fiscal</t>
+  </si>
+  <si>
+    <t>DATE_INCL</t>
+  </si>
+  <si>
+    <t>DATA_ALTER</t>
+  </si>
+  <si>
+    <t>LN_Notas_Operacoes_Fiscais</t>
+  </si>
+  <si>
+    <t>LN_Ordem_Compra_Pre</t>
+  </si>
+  <si>
+    <t>DATA_ORDEM</t>
+  </si>
+  <si>
+    <t>DATA_PLREC</t>
+  </si>
+  <si>
+    <t>DATA_PREREC</t>
+  </si>
+  <si>
+    <t>LN_Pagamento_Titulo</t>
+  </si>
+  <si>
+    <t>DATA_VENC</t>
+  </si>
+  <si>
+    <t>DATA_PAGAM</t>
+  </si>
+  <si>
+    <t>LN_Planejamento e Desenvolvimento - Laudos_e_Etiquetas</t>
+  </si>
+  <si>
+    <t>DATA_OCORRENCIA</t>
+  </si>
+  <si>
+    <t>DATA_NF_ENTRADA</t>
+  </si>
+  <si>
+    <t>COLETA_PREVISTA</t>
+  </si>
+  <si>
+    <t>RETORNO_PREVISTO</t>
+  </si>
+  <si>
+    <t>LN_Planejamento Financeiro - Razão_Contábil</t>
+  </si>
+  <si>
+    <t>DATA_TRANS</t>
+  </si>
+  <si>
+    <t>LN_Planejamento Logístico - Consulta_Ponto_Ent</t>
+  </si>
+  <si>
+    <t>DATA_PONTO</t>
+  </si>
+  <si>
+    <t>DATA_PROCESSAMENTO</t>
+  </si>
+  <si>
+    <t>LN_Planejamento Logístico - Dados_Cliente_Bianca</t>
+  </si>
+  <si>
+    <t>DATA_PROMETIDA</t>
+  </si>
+  <si>
+    <t>LN_Planejamento Logistico - DBO_Painel_Pendentes_Ajustada_Todos</t>
+  </si>
+  <si>
+    <t>DATA_COMPRA</t>
+  </si>
+  <si>
+    <t>LN_Planejamento Logistico -Entregas_Agendadas</t>
+  </si>
+  <si>
+    <t>LN_Planjamento Logístico - Frete_por_Período_e_NF_GTEQ3050</t>
+  </si>
+  <si>
+    <t>DATA_EXPEDICAO</t>
+  </si>
+  <si>
+    <t>DATA_ENTREGA</t>
+  </si>
+  <si>
+    <t>DATA_AJUSTADA</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Colunas1</t>
+  </si>
+  <si>
+    <t>Fábio</t>
+  </si>
+  <si>
+    <t>Colunas2</t>
+  </si>
+  <si>
+    <t>Ronaldo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,13 +404,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -287,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -301,16 +452,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -332,13 +488,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D59" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:D59"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F91" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:F91">
+    <filterColumn colId="4"/>
+    <filterColumn colId="5"/>
+  </autoFilter>
+  <tableColumns count="6">
     <tableColumn id="1" name="View"/>
     <tableColumn id="2" name="Campo"/>
     <tableColumn id="3" name="Tipo de Dados" dataDxfId="1"/>
     <tableColumn id="4" name="Atualização Timezone" dataDxfId="0"/>
+    <tableColumn id="5" name="Colunas1"/>
+    <tableColumn id="6" name="Colunas2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -629,22 +790,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C90" sqref="C90:F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="31.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
+    <row r="1" spans="1:6" ht="18.75">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -657,8 +818,14 @@
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -671,8 +838,11 @@
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -685,8 +855,11 @@
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -699,8 +872,11 @@
       <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -713,8 +889,11 @@
       <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -727,8 +906,11 @@
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -741,8 +923,11 @@
       <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -755,22 +940,29 @@
       <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
+      <c r="E8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="C9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -783,8 +975,11 @@
       <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -797,8 +992,11 @@
       <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -811,8 +1009,11 @@
       <c r="D12" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -825,8 +1026,11 @@
       <c r="D13" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -839,8 +1043,11 @@
       <c r="D14" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -853,8 +1060,11 @@
       <c r="D15" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -867,8 +1077,11 @@
       <c r="D16" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -881,8 +1094,11 @@
       <c r="D17" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -895,8 +1111,11 @@
       <c r="D18" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -909,8 +1128,11 @@
       <c r="D19" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -923,8 +1145,11 @@
       <c r="D20" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -937,8 +1162,11 @@
       <c r="D21" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -951,8 +1179,11 @@
       <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -965,8 +1196,11 @@
       <c r="D23" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -979,8 +1213,11 @@
       <c r="D24" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -993,8 +1230,11 @@
       <c r="D25" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1007,8 +1247,11 @@
       <c r="D26" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1021,8 +1264,11 @@
       <c r="D27" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -1035,8 +1281,11 @@
       <c r="D28" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1049,8 +1298,11 @@
       <c r="D29" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1063,8 +1315,11 @@
       <c r="D30" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -1077,8 +1332,11 @@
       <c r="D31" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1091,8 +1349,11 @@
       <c r="D32" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -1105,8 +1366,11 @@
       <c r="D33" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1119,8 +1383,11 @@
       <c r="D34" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -1133,8 +1400,11 @@
       <c r="D35" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -1147,8 +1417,11 @@
       <c r="D36" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -1161,8 +1434,11 @@
       <c r="D37" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -1175,8 +1451,11 @@
       <c r="D38" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -1189,8 +1468,11 @@
       <c r="D39" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -1203,8 +1485,11 @@
       <c r="D40" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -1217,8 +1502,11 @@
       <c r="D41" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1231,8 +1519,11 @@
       <c r="D42" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -1245,8 +1536,11 @@
       <c r="D43" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -1259,8 +1553,11 @@
       <c r="D44" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -1273,8 +1570,11 @@
       <c r="D45" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -1287,8 +1587,11 @@
       <c r="D46" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -1301,50 +1604,65 @@
       <c r="D47" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" t="s">
+      <c r="E47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" t="s">
+      <c r="C48" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" t="s">
+      <c r="C49" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="C50" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="5" t="s">
         <v>64</v>
       </c>
@@ -1357,8 +1675,11 @@
       <c r="D51" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="5" t="s">
         <v>65</v>
       </c>
@@ -1371,8 +1692,11 @@
       <c r="D52" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="5" t="s">
         <v>67</v>
       </c>
@@ -1385,8 +1709,11 @@
       <c r="D53" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" s="5" t="s">
         <v>69</v>
       </c>
@@ -1399,8 +1726,11 @@
       <c r="D54" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="5" t="s">
         <v>69</v>
       </c>
@@ -1413,8 +1743,11 @@
       <c r="D55" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="E55" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="5" t="s">
         <v>72</v>
       </c>
@@ -1427,8 +1760,11 @@
       <c r="D56" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="E56" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" s="5" t="s">
         <v>72</v>
       </c>
@@ -1441,8 +1777,11 @@
       <c r="D57" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" s="5" t="s">
         <v>74</v>
       </c>
@@ -1455,8 +1794,11 @@
       <c r="D58" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="E58" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" s="5" t="s">
         <v>74</v>
       </c>
@@ -1468,6 +1810,553 @@
       </c>
       <c r="D59" s="6" t="s">
         <v>13</v>
+      </c>
+      <c r="E59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E65" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E66" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E67" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E68" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E69" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E70" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E71" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E72" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E73" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E75" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E77" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E78" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E79" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E80" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E82" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E83" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E84" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E85" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E86" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E87" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E88" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E89" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E90" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E91" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Controle de atualização timezone relatórios
</commit_message>
<xml_diff>
--- a/Relatórios LN/Mapeamento_Reports.xlsx
+++ b/Relatórios LN/Mapeamento_Reports.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="233">
   <si>
     <t>View</t>
   </si>
@@ -653,6 +653,69 @@
   </si>
   <si>
     <t>DATA_ULT_EVENTO</t>
+  </si>
+  <si>
+    <t>DIA</t>
+  </si>
+  <si>
+    <t>DT_SIT</t>
+  </si>
+  <si>
+    <t>DT_LIMITE</t>
+  </si>
+  <si>
+    <t>DT_LIQUIDADO</t>
+  </si>
+  <si>
+    <t>DT_ENTREGA1</t>
+  </si>
+  <si>
+    <t>DT_ULT_EVENTO</t>
+  </si>
+  <si>
+    <t>DT_WMS</t>
+  </si>
+  <si>
+    <t>DT_PROMETIDA</t>
+  </si>
+  <si>
+    <t>PETK_DT_FECHAMENTO_GAIOLA</t>
+  </si>
+  <si>
+    <t>H_ENTRADA,</t>
+  </si>
+  <si>
+    <t>INICIO_EFETIVO,</t>
+  </si>
+  <si>
+    <t>TPREP</t>
+  </si>
+  <si>
+    <t>TREC</t>
+  </si>
+  <si>
+    <t>TTOT</t>
+  </si>
+  <si>
+    <t>DT_APROV</t>
+  </si>
+  <si>
+    <t>DT_REC_HOST</t>
+  </si>
+  <si>
+    <t>DT_FEC_GAI</t>
+  </si>
+  <si>
+    <t>DT_LIQ_SEC</t>
+  </si>
+  <si>
+    <t>DT_EMISSAO_NF</t>
+  </si>
+  <si>
+    <t>WMS_REL_056_ESTOQUE_GERAL_POR_FILIAL</t>
+  </si>
+  <si>
+    <t>DT_SIT_ROM</t>
   </si>
 </sst>
 </file>
@@ -757,7 +820,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -807,8 +870,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F175" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F175">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F211" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F211">
     <filterColumn colId="4"/>
     <filterColumn colId="5"/>
   </autoFilter>
@@ -1109,17 +1172,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F175"/>
+  <dimension ref="A1:F211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D157" sqref="D157"/>
+      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="78.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.140625" style="6" customWidth="1"/>
     <col min="4" max="4" width="31.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" style="5"/>
@@ -3848,97 +3911,139 @@
       <c r="F157" s="14"/>
     </row>
     <row r="158" spans="1:6">
-      <c r="A158" s="17" t="s">
+      <c r="A158" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="B158" s="16"/>
+      <c r="B158" s="16" t="s">
+        <v>154</v>
+      </c>
       <c r="C158" s="15"/>
-      <c r="D158" s="15"/>
-      <c r="E158" s="14"/>
+      <c r="D158" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E158" s="14" t="s">
+        <v>117</v>
+      </c>
       <c r="F158" s="14"/>
     </row>
     <row r="159" spans="1:6">
       <c r="A159" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="B159" s="16"/>
+        <v>185</v>
+      </c>
+      <c r="B159" s="16" t="s">
+        <v>174</v>
+      </c>
       <c r="C159" s="15"/>
-      <c r="D159" s="15"/>
-      <c r="E159" s="14"/>
+      <c r="D159" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E159" s="14" t="s">
+        <v>117</v>
+      </c>
       <c r="F159" s="14"/>
     </row>
     <row r="160" spans="1:6">
       <c r="A160" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="B160" s="16"/>
+        <v>185</v>
+      </c>
+      <c r="B160" s="16" t="s">
+        <v>211</v>
+      </c>
       <c r="C160" s="15"/>
-      <c r="D160" s="15"/>
-      <c r="E160" s="14"/>
+      <c r="D160" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E160" s="14" t="s">
+        <v>117</v>
+      </c>
       <c r="F160" s="14"/>
     </row>
     <row r="161" spans="1:6">
       <c r="A161" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="B161" s="16"/>
+        <v>186</v>
+      </c>
+      <c r="B161" s="16" t="s">
+        <v>205</v>
+      </c>
       <c r="C161" s="15"/>
-      <c r="D161" s="15"/>
-      <c r="E161" s="14"/>
+      <c r="D161" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E161" s="14" t="s">
+        <v>117</v>
+      </c>
       <c r="F161" s="14"/>
     </row>
     <row r="162" spans="1:6">
       <c r="A162" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="B162" s="16"/>
+        <v>186</v>
+      </c>
+      <c r="B162" s="16" t="s">
+        <v>206</v>
+      </c>
       <c r="C162" s="15"/>
-      <c r="D162" s="15"/>
-      <c r="E162" s="14"/>
+      <c r="D162" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E162" s="14" t="s">
+        <v>117</v>
+      </c>
       <c r="F162" s="14"/>
     </row>
     <row r="163" spans="1:6">
       <c r="A163" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="B163" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C163" s="15" t="s">
-        <v>82</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="B163" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="C163" s="15"/>
       <c r="D163" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E163" s="14"/>
+        <v>13</v>
+      </c>
+      <c r="E163" s="14" t="s">
+        <v>117</v>
+      </c>
       <c r="F163" s="14"/>
     </row>
     <row r="164" spans="1:6">
       <c r="A164" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="B164" s="16"/>
+        <v>187</v>
+      </c>
+      <c r="B164" s="16" t="s">
+        <v>206</v>
+      </c>
       <c r="C164" s="15"/>
-      <c r="D164" s="15"/>
-      <c r="E164" s="14"/>
+      <c r="D164" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E164" s="14" t="s">
+        <v>117</v>
+      </c>
       <c r="F164" s="14"/>
     </row>
     <row r="165" spans="1:6">
       <c r="A165" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="B165" s="16"/>
+        <v>188</v>
+      </c>
+      <c r="B165" s="16" t="s">
+        <v>212</v>
+      </c>
       <c r="C165" s="15"/>
-      <c r="D165" s="15"/>
-      <c r="E165" s="14"/>
-      <c r="F165" s="12"/>
-    </row>
-    <row r="166" spans="1:6" ht="30">
+      <c r="D165" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E165" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F165" s="14"/>
+    </row>
+    <row r="166" spans="1:6">
       <c r="A166" s="14" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B166" s="16" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C166" s="15"/>
       <c r="D166" s="15" t="s">
@@ -3947,125 +4052,736 @@
       <c r="E166" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="F166" s="12"/>
+      <c r="F166" s="14"/>
     </row>
     <row r="167" spans="1:6">
       <c r="A167" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="B167" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="C167" s="15"/>
+      <c r="D167" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E167" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F167" s="14"/>
+    </row>
+    <row r="168" spans="1:6">
+      <c r="A168" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B168" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C168" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D168" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E168" s="14"/>
+      <c r="F168" s="14"/>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="A169" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="B169" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="C169" s="15"/>
+      <c r="D169" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E169" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F169" s="14"/>
+    </row>
+    <row r="170" spans="1:6">
+      <c r="A170" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="B170" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="C170" s="15"/>
+      <c r="D170" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E170" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F170" s="14"/>
+    </row>
+    <row r="171" spans="1:6">
+      <c r="A171" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="B171" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="C171" s="15"/>
+      <c r="D171" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E171" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F171" s="12"/>
+    </row>
+    <row r="172" spans="1:6">
+      <c r="A172" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="B172" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="C172" s="15"/>
+      <c r="D172" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E172" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F172" s="12"/>
+    </row>
+    <row r="173" spans="1:6" ht="30">
+      <c r="A173" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="B173" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="C173" s="15"/>
+      <c r="D173" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E173" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F173" s="12"/>
+    </row>
+    <row r="174" spans="1:6">
+      <c r="A174" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="B167" s="15" t="s">
+      <c r="B174" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D174" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E174" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F174" s="12"/>
+    </row>
+    <row r="175" spans="1:6">
+      <c r="A175" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="B175" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="C167" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D167" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E167" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="F167" s="12"/>
-    </row>
-    <row r="168" spans="1:6">
-      <c r="A168" s="12" t="s">
+      <c r="C175" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D175" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E175" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F175" s="12"/>
+    </row>
+    <row r="176" spans="1:6">
+      <c r="A176" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="B176" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C176" s="15"/>
+      <c r="D176" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E176" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F176" s="12"/>
+    </row>
+    <row r="177" spans="1:6">
+      <c r="A177" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="B177" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C177" s="15"/>
+      <c r="D177" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E177" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F177" s="12"/>
+    </row>
+    <row r="178" spans="1:6">
+      <c r="A178" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="B178" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="C178" s="15"/>
+      <c r="D178" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E178" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F178" s="12"/>
+    </row>
+    <row r="179" spans="1:6">
+      <c r="A179" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="B179" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C179" s="15"/>
+      <c r="D179" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E179" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F179" s="12"/>
+    </row>
+    <row r="180" spans="1:6">
+      <c r="A180" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="B168" s="16"/>
-      <c r="C168" s="13"/>
-      <c r="D168" s="13"/>
-      <c r="E168" s="12"/>
-      <c r="F168" s="12"/>
-    </row>
-    <row r="169" spans="1:6">
-      <c r="A169" s="12" t="s">
+      <c r="B180" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="C180" s="13"/>
+      <c r="D180" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E180" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F180" s="12"/>
+    </row>
+    <row r="181" spans="1:6">
+      <c r="A181" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="B181" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="C181" s="13"/>
+      <c r="D181" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E181" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F181" s="12"/>
+    </row>
+    <row r="182" spans="1:6">
+      <c r="A182" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="B182" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="C182" s="13"/>
+      <c r="D182" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E182" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F182" s="12"/>
+    </row>
+    <row r="183" spans="1:6">
+      <c r="A183" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="B183" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="C183" s="13"/>
+      <c r="D183" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E183" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F183" s="12"/>
+    </row>
+    <row r="184" spans="1:6">
+      <c r="A184" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="B184" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="C184" s="13"/>
+      <c r="D184" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E184" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F184" s="12"/>
+    </row>
+    <row r="185" spans="1:6">
+      <c r="A185" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="B169" s="15" t="s">
+      <c r="B185" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C169" s="15" t="s">
+      <c r="C185" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D169" s="15" t="s">
+      <c r="D185" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="E169" s="14"/>
-      <c r="F169" s="12"/>
-    </row>
-    <row r="170" spans="1:6">
-      <c r="A170" s="12" t="s">
+      <c r="E185" s="14"/>
+      <c r="F185" s="12"/>
+    </row>
+    <row r="186" spans="1:6">
+      <c r="A186" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="B170" s="16"/>
-      <c r="C170" s="13"/>
-      <c r="D170" s="13"/>
-      <c r="E170" s="12"/>
-      <c r="F170" s="12"/>
-    </row>
-    <row r="171" spans="1:6">
-      <c r="A171" s="12" t="s">
+      <c r="B186" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="C186" s="13"/>
+      <c r="D186" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E186" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F186" s="12"/>
+    </row>
+    <row r="187" spans="1:6">
+      <c r="A187" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="B187" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C187" s="13"/>
+      <c r="D187" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E187" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F187" s="12"/>
+    </row>
+    <row r="188" spans="1:6">
+      <c r="A188" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="B188" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="C188" s="13"/>
+      <c r="D188" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E188" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F188" s="12"/>
+    </row>
+    <row r="189" spans="1:6">
+      <c r="A189" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="B189" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="C189" s="13"/>
+      <c r="D189" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E189" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F189" s="12"/>
+    </row>
+    <row r="190" spans="1:6">
+      <c r="A190" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="B190" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="C190" s="13"/>
+      <c r="D190" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E190" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F190" s="12"/>
+    </row>
+    <row r="191" spans="1:6">
+      <c r="A191" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="B171" s="16"/>
-      <c r="C171" s="13"/>
-      <c r="D171" s="13"/>
-      <c r="E171" s="12"/>
-      <c r="F171" s="12"/>
-    </row>
-    <row r="172" spans="1:6">
-      <c r="A172" s="12" t="s">
+      <c r="B191" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="C191" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D191" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E191" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F191" s="12"/>
+    </row>
+    <row r="192" spans="1:6">
+      <c r="A192" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B192" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="C192" s="13"/>
+      <c r="D192" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E192" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F192" s="12"/>
+    </row>
+    <row r="193" spans="1:6">
+      <c r="A193" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B193" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="C193" s="13"/>
+      <c r="D193" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E193" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F193" s="12"/>
+    </row>
+    <row r="194" spans="1:6">
+      <c r="A194" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B194" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="C194" s="13"/>
+      <c r="D194" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E194" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F194" s="12"/>
+    </row>
+    <row r="195" spans="1:6">
+      <c r="A195" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B195" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="C195" s="13"/>
+      <c r="D195" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E195" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F195" s="12"/>
+    </row>
+    <row r="196" spans="1:6">
+      <c r="A196" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B196" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="C196" s="13"/>
+      <c r="D196" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E196" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F196" s="12"/>
+    </row>
+    <row r="197" spans="1:6">
+      <c r="A197" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B197" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="C197" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D197" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E197" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F197" s="12"/>
+    </row>
+    <row r="198" spans="1:6">
+      <c r="A198" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="B172" s="16"/>
-      <c r="C172" s="13"/>
-      <c r="D172" s="13"/>
-      <c r="E172" s="12"/>
-      <c r="F172" s="12"/>
-    </row>
-    <row r="173" spans="1:6">
-      <c r="A173" s="12" t="s">
+      <c r="B198" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C198" s="13"/>
+      <c r="D198" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E198" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F198" s="12"/>
+    </row>
+    <row r="199" spans="1:6">
+      <c r="A199" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="B199" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="C199" s="13"/>
+      <c r="D199" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E199" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F199" s="12"/>
+    </row>
+    <row r="200" spans="1:6">
+      <c r="A200" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B200" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C200" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D200" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E200" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F200" s="12"/>
+    </row>
+    <row r="201" spans="1:6">
+      <c r="A201" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="B173" s="15" t="s">
+      <c r="B201" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="C173" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D173" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E173" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="F173" s="12"/>
-    </row>
-    <row r="174" spans="1:6">
-      <c r="A174" s="12" t="s">
+      <c r="C201" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D201" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E201" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F201" s="12"/>
+    </row>
+    <row r="202" spans="1:6">
+      <c r="A202" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="B202" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C202" s="15"/>
+      <c r="D202" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E202" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F202" s="12"/>
+    </row>
+    <row r="203" spans="1:6">
+      <c r="A203" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="B203" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C203" s="15"/>
+      <c r="D203" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E203" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F203" s="12"/>
+    </row>
+    <row r="204" spans="1:6">
+      <c r="A204" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="B204" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="C204" s="15"/>
+      <c r="D204" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E204" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F204" s="12"/>
+    </row>
+    <row r="205" spans="1:6">
+      <c r="A205" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="B205" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C205" s="15"/>
+      <c r="D205" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E205" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F205" s="12"/>
+    </row>
+    <row r="206" spans="1:6">
+      <c r="A206" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="B174" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C174" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D174" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E174" s="14"/>
-      <c r="F174" s="14"/>
-    </row>
-    <row r="175" spans="1:6">
-      <c r="A175" s="12" t="s">
+      <c r="B206" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="C206" s="15"/>
+      <c r="D206" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E206" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F206" s="12"/>
+    </row>
+    <row r="207" spans="1:6">
+      <c r="A207" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="B175" s="16"/>
-      <c r="C175" s="13"/>
-      <c r="D175" s="13"/>
-      <c r="E175" s="12"/>
-      <c r="F175" s="12"/>
+      <c r="B207" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C207" s="15"/>
+      <c r="D207" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E207" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F207" s="12"/>
+    </row>
+    <row r="208" spans="1:6">
+      <c r="A208" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B208" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C208" s="15"/>
+      <c r="D208" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E208" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F208" s="14"/>
+    </row>
+    <row r="209" spans="1:6">
+      <c r="A209" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B209" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="C209" s="13"/>
+      <c r="D209" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E209" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F209" s="12"/>
+    </row>
+    <row r="210" spans="1:6">
+      <c r="A210" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B210" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="C210" s="13"/>
+      <c r="D210" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E210" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F210" s="12"/>
+    </row>
+    <row r="211" spans="1:6">
+      <c r="A211" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B211" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="C211" s="13"/>
+      <c r="D211" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E211" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F211" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>